<commit_message>
commiting with new project file
</commit_message>
<xml_diff>
--- a/InputFiles/TC02_Bento_LocalSearch-UploadCaseSet_Enter_CASEID_List.xlsx
+++ b/InputFiles/TC02_Bento_LocalSearch-UploadCaseSet_Enter_CASEID_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781D6252-56AF-476E-88D8-E35A215244BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72475BFA-83B2-4897-8F53-CFAD9E7A468F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11145" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>WebExcel</t>
   </si>
@@ -45,18 +45,47 @@
     <t>StatQuery</t>
   </si>
   <si>
-    <t>TabName</t>
-  </si>
-  <si>
     <t>CasesTab</t>
   </si>
   <si>
+    <t>TC02_Bento_LocalSearch-UploadCaseSet_Enter_CASEID_List_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC02_Bento_LocalSearch-UploadCaseSet_Enter_CASEID_List_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>TC02_Bento_LocalSearch-UploadCaseSet_Enter_CASEID_List</t>
+  </si>
+  <si>
     <t>MATCH (ss:study_subject)
+MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
+WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
+MATCH (ss:study_subject)
+	WHERE ss.study_subject_id = 'BENTO-CASE-3405467'
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
+MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
+MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
+MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
+RETURN DISTINCT 
+	ss.study_subject_id AS `Case ID`,
+	p.program_acronym AS `Program Code`,
+	p.program_id AS `Program ID`,
+	s.study_acronym AS `Arm`,
+	ss.disease_subtype AS `Diagnosis`,
+	sf.grouped_recurrence_score AS `Recurrence Score`,
+	d.tumor_size_group AS `Tumor Size (cm)`,
+	d.er_status AS `ER Status`,
+	d.pr_status AS `PR Status`,
+	demo.age_at_index AS `Age (years)`,
+	demo.survival_time AS `Survival (days)`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (ss:study_subject)
 MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-WHERE    d.er_status IN ["Positive"] 
 MATCH (ss)-[:study_subject_of_study]-&gt;(s)
+WHERE ss.study_subject_id = 'BENTO-CASE-3405467'
 MATCH (s)-[:study_of_program]-&gt;(p)
 MATCH (ss)&lt;-[:sample_of_study_subject]-(samp)
 MATCH (samp)&lt;-[:file_of_sample]-(f)
@@ -66,35 +95,50 @@
 COUNT(DISTINCT ss) AS Cases,
 COUNT(DISTINCT samp) AS Samples,
 COUNT(DISTINCT lp) AS Assays,
-COUNT(DISTINCT f) AS Files</t>
+COUNT(DISTINCT f) AS Files
+</t>
+  </si>
+  <si>
+    <t>SamplesTab</t>
   </si>
   <si>
     <t>MATCH (ss:study_subject)
-MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
-WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
+	WHERE ss.study_subject_id = 'BENTO-CASE-3405467'
+MATCH (ss)&lt;-[:sample_of_study_subject]-(samp)
 MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
-MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
-MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
-MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
- WHERE   d.er_status IN ["Positive"] 
-return ss.study_subject_id as `Case ID`,
-       p.program_acronym as `Program Code`,
-        p.program_id as Program_ID,
-       s.study_acronym as `Arm`,
-       ss.disease_subtype as `Diagnosis`,
-       sf.grouped_recurrence_score AS `Recurrence Score`,
-       d.tumor_size_group AS `tumor_size`,
-       d.er_status AS `ER Status`,
-       d.pr_status AS `PR Status`,
-       demo.age_at_index AS `Age (years)`,
-demo.survival_time AS `Survival (days)`</t>
-  </si>
-  <si>
-    <t>TC02_Bento_LocalSearch-UploadCaseSet_Enter_CASEID_List_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC02_Bento_LocalSearch-UploadCaseSet_Enter_CASEID_List_WebData.xlsx</t>
+MATCH (ss)&lt;-[*..2]-(parent)&lt;--(f:file)
+OPTIONAL MATCH (f)-[:file_of_laboratory_procedure]-&gt;(lp)
+RETURN DISTINCT 
+	samp.sample_id AS `Sample ID`,
+	ss.study_subject_id AS `Case ID`,
+	p.program_acronym AS `Program Code`,
+	s.study_acronym AS `Arm`,
+	ss.disease_subtype AS `Diagnosis`,
+	samp.tissue_type AS `Tissue Type`,
+	samp.composition AS `Tissue Composition`,
+	samp.sample_anatomic_site AS `Sample Anatomic Site`,
+	samp.method_of_sample_procurement AS `Sample Procurement Method`,
+	lp.test_name AS `platform`</t>
+  </si>
+  <si>
+    <t>FilesTab</t>
+  </si>
+  <si>
+    <t>MATCH (ss:study_subject)
+	WHERE ss.study_subject_id = 'BENTO-CASE-3405467'
+MATCH (ss)&lt;-[*..2]-(parent)&lt;--(f:file)
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
+MATCH (ss)&lt;-[:sample_of_study_subject]-(samp)
+RETURN DISTINCT 
+	f.file_name AS `File Name`,
+	head(labels(parent)) AS `Association`,
+	f.file_description AS `Description`,
+	f.file_format AS `File Format`,
+	f.file_size AS `Size`,
+	p.program_acronym AS `Program Code`,
+	s.study_acronym AS `Arm`,
+	ss.study_subject_id AS `Case ID`,
+	samp.sample_id AS `Sample ID`</t>
   </si>
 </sst>
 </file>
@@ -464,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +525,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -496,21 +540,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="330" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="345" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="255" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="255" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>